<commit_message>
feat: Ajustar dados de acordo com uma linha especifica
</commit_message>
<xml_diff>
--- a/test/cypress/fixtures/teste-xls-cypress.xlsx
+++ b/test/cypress/fixtures/teste-xls-cypress.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+  <si>
+    <t>Mês</t>
+  </si>
   <si>
     <t>Pensamento</t>
   </si>
@@ -22,13 +25,37 @@
     <t>Modelo</t>
   </si>
   <si>
-    <t>Teste de pensamento</t>
+    <t>Default</t>
   </si>
   <si>
     <t>Cypress</t>
   </si>
   <si>
+    <t>Modelo 1</t>
+  </si>
+  <si>
+    <t>Mês 1</t>
+  </si>
+  <si>
+    <t>Mês 2</t>
+  </si>
+  <si>
+    <t>Modelo 2</t>
+  </si>
+  <si>
+    <t>Mês 3</t>
+  </si>
+  <si>
+    <t>Mês 4</t>
+  </si>
+  <si>
     <t>Modelo 3</t>
+  </si>
+  <si>
+    <t>Mês 5</t>
+  </si>
+  <si>
+    <t>Mês 6</t>
   </si>
 </sst>
 </file>
@@ -87,10 +114,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -309,6 +336,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="18.13"/>
+    <col customWidth="1" min="2" max="2" width="16.38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -321,16 +349,106 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" s="2">
+        <v>0.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>